<commit_message>
Avance en puntos de historial
</commit_message>
<xml_diff>
--- a/Cap. Esp..xlsx
+++ b/Cap. Esp..xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gesse\OneDrive\Escritorio\RCC\RCC V7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u86427\Desktop\Guillermo\Python\MERP\Django\RCC\RCC\RCC V7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3D2541-AE87-47E1-BCB4-57F81C6E5BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$E$2:$F$225</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -477,7 +476,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -535,6 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,21 +814,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="207" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="150.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -852,7 +852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -876,7 +876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>34</v>
       </c>
@@ -899,7 +899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>35</v>
       </c>
@@ -922,7 +922,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>36</v>
       </c>
@@ -945,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>37</v>
       </c>
@@ -968,7 +968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>38</v>
       </c>
@@ -991,7 +991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>39</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>40</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41</v>
       </c>
@@ -1056,11 +1056,11 @@
         <v>199</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f>LEN(C10)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>42</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>43</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>45</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>46</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>47</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>48</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>49</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>50</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>51</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>52</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>53</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>54</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>55</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>56</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>57</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>58</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>59</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>60</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>61</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>62</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>63</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>64</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>65</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>66</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>67</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>68</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>69</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>70</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>71</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>72</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>73</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>74</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>75</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>76</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>77</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>78</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>79</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>80</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>81</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>82</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>83</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>84</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>85</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>86</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>87</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>88</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>89</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>90</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>91</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>92</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>93</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>94</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>95</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>96</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>97</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>98</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>99</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>100</v>
       </c>
@@ -2421,6 +2421,627 @@
       <c r="G69">
         <f t="shared" si="3"/>
         <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C76" s="7">
+        <v>1</v>
+      </c>
+      <c r="D76" t="str">
+        <f>C76&amp;": hab_esp_"&amp;C76&amp;","</f>
+        <v>1: hab_esp_1,</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C77" s="7">
+        <v>26</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" ref="D77:D140" si="6">C77&amp;": hab_esp_"&amp;C77&amp;","</f>
+        <v>26: hab_esp_26,</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C78" s="7">
+        <v>34</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="6"/>
+        <v>34: hab_esp_34,</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C79" s="7">
+        <v>35</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="6"/>
+        <v>35: hab_esp_35,</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C80" s="7">
+        <v>36</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="6"/>
+        <v>36: hab_esp_36,</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="7">
+        <v>37</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="6"/>
+        <v>37: hab_esp_37,</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="7">
+        <v>38</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="6"/>
+        <v>38: hab_esp_38,</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="7">
+        <v>39</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="6"/>
+        <v>39: hab_esp_39,</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="7">
+        <v>40</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="6"/>
+        <v>40: hab_esp_40,</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="7">
+        <v>41</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="6"/>
+        <v>41: hab_esp_41,</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="7">
+        <v>42</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="6"/>
+        <v>42: hab_esp_42,</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="7">
+        <v>43</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="6"/>
+        <v>43: hab_esp_43,</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="7">
+        <v>44</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="6"/>
+        <v>44: hab_esp_44,</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="7">
+        <v>45</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="6"/>
+        <v>45: hab_esp_45,</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="7">
+        <v>46</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="6"/>
+        <v>46: hab_esp_46,</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="7">
+        <v>47</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="6"/>
+        <v>47: hab_esp_47,</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="7">
+        <v>48</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="6"/>
+        <v>48: hab_esp_48,</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="7">
+        <v>49</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="6"/>
+        <v>49: hab_esp_49,</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="7">
+        <v>50</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="6"/>
+        <v>50: hab_esp_50,</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95" s="7">
+        <v>51</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="6"/>
+        <v>51: hab_esp_51,</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="7">
+        <v>52</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="6"/>
+        <v>52: hab_esp_52,</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="7">
+        <v>53</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="6"/>
+        <v>53: hab_esp_53,</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="7">
+        <v>54</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="6"/>
+        <v>54: hab_esp_54,</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="7">
+        <v>55</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="6"/>
+        <v>55: hab_esp_55,</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="7">
+        <v>56</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="6"/>
+        <v>56: hab_esp_56,</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="7">
+        <v>57</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="6"/>
+        <v>57: hab_esp_57,</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="7">
+        <v>58</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="6"/>
+        <v>58: hab_esp_58,</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="7">
+        <v>59</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="6"/>
+        <v>59: hab_esp_59,</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="7">
+        <v>60</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="6"/>
+        <v>60: hab_esp_60,</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="7">
+        <v>61</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="6"/>
+        <v>61: hab_esp_61,</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="7">
+        <v>62</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="6"/>
+        <v>62: hab_esp_62,</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="7">
+        <v>63</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="6"/>
+        <v>63: hab_esp_63,</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="7">
+        <v>64</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="6"/>
+        <v>64: hab_esp_64,</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="7">
+        <v>65</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="6"/>
+        <v>65: hab_esp_65,</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="7">
+        <v>66</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="6"/>
+        <v>66: hab_esp_66,</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C111" s="7">
+        <v>67</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="6"/>
+        <v>67: hab_esp_67,</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="7">
+        <v>68</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="6"/>
+        <v>68: hab_esp_68,</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="7">
+        <v>69</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="6"/>
+        <v>69: hab_esp_69,</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="7">
+        <v>70</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="6"/>
+        <v>70: hab_esp_70,</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="7">
+        <v>71</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="6"/>
+        <v>71: hab_esp_71,</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="7">
+        <v>72</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="6"/>
+        <v>72: hab_esp_72,</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="7">
+        <v>73</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="6"/>
+        <v>73: hab_esp_73,</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="7">
+        <v>74</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="6"/>
+        <v>74: hab_esp_74,</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="7">
+        <v>75</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="6"/>
+        <v>75: hab_esp_75,</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" s="7">
+        <v>76</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="6"/>
+        <v>76: hab_esp_76,</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="7">
+        <v>77</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="6"/>
+        <v>77: hab_esp_77,</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="7">
+        <v>78</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="6"/>
+        <v>78: hab_esp_78,</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="7">
+        <v>79</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="6"/>
+        <v>79: hab_esp_79,</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="7">
+        <v>80</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="6"/>
+        <v>80: hab_esp_80,</v>
+      </c>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="7">
+        <v>81</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="6"/>
+        <v>81: hab_esp_81,</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="7">
+        <v>82</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="6"/>
+        <v>82: hab_esp_82,</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="7">
+        <v>83</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="6"/>
+        <v>83: hab_esp_83,</v>
+      </c>
+    </row>
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C128" s="7">
+        <v>84</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="6"/>
+        <v>84: hab_esp_84,</v>
+      </c>
+    </row>
+    <row r="129" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C129" s="7">
+        <v>85</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="6"/>
+        <v>85: hab_esp_85,</v>
+      </c>
+    </row>
+    <row r="130" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C130" s="7">
+        <v>86</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="6"/>
+        <v>86: hab_esp_86,</v>
+      </c>
+    </row>
+    <row r="131" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C131" s="7">
+        <v>87</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="6"/>
+        <v>87: hab_esp_87,</v>
+      </c>
+    </row>
+    <row r="132" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C132" s="7">
+        <v>88</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="6"/>
+        <v>88: hab_esp_88,</v>
+      </c>
+    </row>
+    <row r="133" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C133" s="7">
+        <v>89</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="6"/>
+        <v>89: hab_esp_89,</v>
+      </c>
+    </row>
+    <row r="134" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C134" s="7">
+        <v>90</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="6"/>
+        <v>90: hab_esp_90,</v>
+      </c>
+    </row>
+    <row r="135" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C135" s="7">
+        <v>91</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="6"/>
+        <v>91: hab_esp_91,</v>
+      </c>
+    </row>
+    <row r="136" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C136" s="7">
+        <v>92</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="6"/>
+        <v>92: hab_esp_92,</v>
+      </c>
+    </row>
+    <row r="137" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C137" s="7">
+        <v>93</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="6"/>
+        <v>93: hab_esp_93,</v>
+      </c>
+    </row>
+    <row r="138" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C138" s="7">
+        <v>94</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="6"/>
+        <v>94: hab_esp_94,</v>
+      </c>
+    </row>
+    <row r="139" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C139" s="7">
+        <v>95</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="6"/>
+        <v>95: hab_esp_95,</v>
+      </c>
+    </row>
+    <row r="140" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C140" s="7">
+        <v>96</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="6"/>
+        <v>96: hab_esp_96,</v>
+      </c>
+    </row>
+    <row r="141" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C141" s="7">
+        <v>97</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" ref="D141:D144" si="7">C141&amp;": hab_esp_"&amp;C141&amp;","</f>
+        <v>97: hab_esp_97,</v>
+      </c>
+    </row>
+    <row r="142" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C142" s="7">
+        <v>98</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="7"/>
+        <v>98: hab_esp_98,</v>
+      </c>
+    </row>
+    <row r="143" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C143" s="7">
+        <v>99</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="7"/>
+        <v>99: hab_esp_99,</v>
+      </c>
+    </row>
+    <row r="144" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C144" s="7">
+        <v>100</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="7"/>
+        <v>100: hab_esp_100,</v>
       </c>
     </row>
   </sheetData>
@@ -2430,16 +3051,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E82D6E-79FB-4501-BC6E-470E9C5171A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F225"/>
   <sheetViews>
     <sheetView topLeftCell="A163" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>141</v>
       </c>
@@ -2454,7 +3075,7 @@
         <v>def hab_esp_35(dato, personaje):</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>140</v>
       </c>
@@ -2463,7 +3084,7 @@
         <v>    return</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>36</v>
       </c>
@@ -2472,7 +3093,7 @@
         <v>def hab_esp_36(dato, personaje):</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>143</v>
       </c>
@@ -2481,12 +3102,12 @@
         <v>    return</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E8">
         <f>E5+1</f>
         <v>37</v>
@@ -2496,15 +3117,15 @@
         <v>def hab_esp_37(dato, personaje):</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F9" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E11">
-        <f t="shared" ref="E9:E72" si="0">E8+1</f>
+        <f t="shared" ref="E11:E71" si="0">E8+1</f>
         <v>38</v>
       </c>
       <c r="F11" t="str">
@@ -2512,13 +3133,13 @@
         <v>def hab_esp_38(dato, personaje):</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F12" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E14">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2528,13 +3149,13 @@
         <v>def hab_esp_39(dato, personaje):</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F15" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2544,13 +3165,13 @@
         <v>def hab_esp_40(dato, personaje):</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F18" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2560,13 +3181,13 @@
         <v>def hab_esp_41(dato, personaje):</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F21" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2576,13 +3197,13 @@
         <v>def hab_esp_42(dato, personaje):</v>
       </c>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F24" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2592,13 +3213,13 @@
         <v>def hab_esp_43(dato, personaje):</v>
       </c>
     </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F27" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E29">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2608,13 +3229,13 @@
         <v>def hab_esp_44(dato, personaje):</v>
       </c>
     </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F30" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E32">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2624,13 +3245,13 @@
         <v>def hab_esp_45(dato, personaje):</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F33" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E35">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2640,13 +3261,13 @@
         <v>def hab_esp_46(dato, personaje):</v>
       </c>
     </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F36" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E38">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2656,13 +3277,13 @@
         <v>def hab_esp_47(dato, personaje):</v>
       </c>
     </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F39" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E41">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2672,13 +3293,13 @@
         <v>def hab_esp_48(dato, personaje):</v>
       </c>
     </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F42" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E44">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2688,13 +3309,13 @@
         <v>def hab_esp_49(dato, personaje):</v>
       </c>
     </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F45" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E47">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2704,13 +3325,13 @@
         <v>def hab_esp_50(dato, personaje):</v>
       </c>
     </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F48" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2720,13 +3341,13 @@
         <v>def hab_esp_51(dato, personaje):</v>
       </c>
     </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F51" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E53">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2736,13 +3357,13 @@
         <v>def hab_esp_52(dato, personaje):</v>
       </c>
     </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F54" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E56">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2752,13 +3373,13 @@
         <v>def hab_esp_53(dato, personaje):</v>
       </c>
     </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F57" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E59">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2768,13 +3389,13 @@
         <v>def hab_esp_54(dato, personaje):</v>
       </c>
     </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F60" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E62">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -2784,13 +3405,13 @@
         <v>def hab_esp_55(dato, personaje):</v>
       </c>
     </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F63" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2800,13 +3421,13 @@
         <v>def hab_esp_56(dato, personaje):</v>
       </c>
     </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F66" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E68">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2816,13 +3437,13 @@
         <v>def hab_esp_57(dato, personaje):</v>
       </c>
     </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F69" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2832,15 +3453,15 @@
         <v>def hab_esp_58(dato, personaje):</v>
       </c>
     </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F72" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74">
-        <f t="shared" ref="E73:E136" si="1">E71+1</f>
+        <f t="shared" ref="E74:E134" si="1">E71+1</f>
         <v>59</v>
       </c>
       <c r="F74" t="str">
@@ -2848,13 +3469,13 @@
         <v>def hab_esp_59(dato, personaje):</v>
       </c>
     </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F75" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E77">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2864,13 +3485,13 @@
         <v>def hab_esp_60(dato, personaje):</v>
       </c>
     </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F78" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E80">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2880,13 +3501,13 @@
         <v>def hab_esp_61(dato, personaje):</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F81" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2896,13 +3517,13 @@
         <v>def hab_esp_62(dato, personaje):</v>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F84" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2912,13 +3533,13 @@
         <v>def hab_esp_63(dato, personaje):</v>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F87" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2928,13 +3549,13 @@
         <v>def hab_esp_64(dato, personaje):</v>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F90" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E92">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -2944,13 +3565,13 @@
         <v>def hab_esp_65(dato, personaje):</v>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F93" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -2960,13 +3581,13 @@
         <v>def hab_esp_66(dato, personaje):</v>
       </c>
     </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F96" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E98">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -2976,13 +3597,13 @@
         <v>def hab_esp_67(dato, personaje):</v>
       </c>
     </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F99" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E101">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -2992,13 +3613,13 @@
         <v>def hab_esp_68(dato, personaje):</v>
       </c>
     </row>
-    <row r="102" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F102" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="104" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E104">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -3008,13 +3629,13 @@
         <v>def hab_esp_69(dato, personaje):</v>
       </c>
     </row>
-    <row r="105" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F105" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="107" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E107">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -3024,13 +3645,13 @@
         <v>def hab_esp_70(dato, personaje):</v>
       </c>
     </row>
-    <row r="108" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F108" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="110" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E110">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -3040,13 +3661,13 @@
         <v>def hab_esp_71(dato, personaje):</v>
       </c>
     </row>
-    <row r="111" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F111" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E113">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3056,13 +3677,13 @@
         <v>def hab_esp_72(dato, personaje):</v>
       </c>
     </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F114" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E116">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -3072,13 +3693,13 @@
         <v>def hab_esp_73(dato, personaje):</v>
       </c>
     </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F117" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E119">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -3088,13 +3709,13 @@
         <v>def hab_esp_74(dato, personaje):</v>
       </c>
     </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F120" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E122">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -3104,13 +3725,13 @@
         <v>def hab_esp_75(dato, personaje):</v>
       </c>
     </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F123" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E125">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -3120,13 +3741,13 @@
         <v>def hab_esp_76(dato, personaje):</v>
       </c>
     </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F126" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E128">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -3136,13 +3757,13 @@
         <v>def hab_esp_77(dato, personaje):</v>
       </c>
     </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F129" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E131">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -3152,13 +3773,13 @@
         <v>def hab_esp_78(dato, personaje):</v>
       </c>
     </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F132" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E134">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -3168,13 +3789,13 @@
         <v>def hab_esp_79(dato, personaje):</v>
       </c>
     </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F135" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E137">
         <f t="shared" ref="E137:E200" si="2">E134+1</f>
         <v>80</v>
@@ -3184,13 +3805,13 @@
         <v>def hab_esp_80(dato, personaje):</v>
       </c>
     </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F138" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E140">
         <f t="shared" si="2"/>
         <v>81</v>
@@ -3200,13 +3821,13 @@
         <v>def hab_esp_81(dato, personaje):</v>
       </c>
     </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F141" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="143" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E143">
         <f t="shared" si="2"/>
         <v>82</v>
@@ -3216,13 +3837,13 @@
         <v>def hab_esp_82(dato, personaje):</v>
       </c>
     </row>
-    <row r="144" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F144" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="146" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E146">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -3232,13 +3853,13 @@
         <v>def hab_esp_83(dato, personaje):</v>
       </c>
     </row>
-    <row r="147" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F147" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="149" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E149">
         <f t="shared" si="2"/>
         <v>84</v>
@@ -3248,13 +3869,13 @@
         <v>def hab_esp_84(dato, personaje):</v>
       </c>
     </row>
-    <row r="150" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F150" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="152" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E152">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -3264,13 +3885,13 @@
         <v>def hab_esp_85(dato, personaje):</v>
       </c>
     </row>
-    <row r="153" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F153" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="155" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E155">
         <f t="shared" si="2"/>
         <v>86</v>
@@ -3280,13 +3901,13 @@
         <v>def hab_esp_86(dato, personaje):</v>
       </c>
     </row>
-    <row r="156" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F156" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="158" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E158">
         <f t="shared" si="2"/>
         <v>87</v>
@@ -3296,13 +3917,13 @@
         <v>def hab_esp_87(dato, personaje):</v>
       </c>
     </row>
-    <row r="159" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F159" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="161" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E161">
         <f t="shared" si="2"/>
         <v>88</v>
@@ -3312,13 +3933,13 @@
         <v>def hab_esp_88(dato, personaje):</v>
       </c>
     </row>
-    <row r="162" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F162" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="164" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E164">
         <f t="shared" si="2"/>
         <v>89</v>
@@ -3328,13 +3949,13 @@
         <v>def hab_esp_89(dato, personaje):</v>
       </c>
     </row>
-    <row r="165" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F165" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="167" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E167">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -3344,13 +3965,13 @@
         <v>def hab_esp_90(dato, personaje):</v>
       </c>
     </row>
-    <row r="168" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F168" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="170" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E170">
         <f t="shared" si="2"/>
         <v>91</v>
@@ -3360,13 +3981,13 @@
         <v>def hab_esp_91(dato, personaje):</v>
       </c>
     </row>
-    <row r="171" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F171" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="173" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E173">
         <f t="shared" si="2"/>
         <v>92</v>
@@ -3376,13 +3997,13 @@
         <v>def hab_esp_92(dato, personaje):</v>
       </c>
     </row>
-    <row r="174" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F174" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="176" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E176">
         <f t="shared" si="2"/>
         <v>93</v>
@@ -3392,13 +4013,13 @@
         <v>def hab_esp_93(dato, personaje):</v>
       </c>
     </row>
-    <row r="177" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F177" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="179" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E179">
         <f t="shared" si="2"/>
         <v>94</v>
@@ -3408,13 +4029,13 @@
         <v>def hab_esp_94(dato, personaje):</v>
       </c>
     </row>
-    <row r="180" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F180" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="182" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E182">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -3424,13 +4045,13 @@
         <v>def hab_esp_95(dato, personaje):</v>
       </c>
     </row>
-    <row r="183" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F183" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="185" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E185">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -3440,13 +4061,13 @@
         <v>def hab_esp_96(dato, personaje):</v>
       </c>
     </row>
-    <row r="186" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F186" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="188" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E188">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -3456,13 +4077,13 @@
         <v>def hab_esp_97(dato, personaje):</v>
       </c>
     </row>
-    <row r="189" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F189" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="191" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E191">
         <f t="shared" si="2"/>
         <v>98</v>
@@ -3472,13 +4093,13 @@
         <v>def hab_esp_98(dato, personaje):</v>
       </c>
     </row>
-    <row r="192" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F192" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="194" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E194">
         <f t="shared" si="2"/>
         <v>99</v>
@@ -3488,13 +4109,13 @@
         <v>def hab_esp_99(dato, personaje):</v>
       </c>
     </row>
-    <row r="195" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F195" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="197" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E197">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -3504,13 +4125,13 @@
         <v>def hab_esp_100(dato, personaje):</v>
       </c>
     </row>
-    <row r="198" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F198" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="200" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E200">
         <f t="shared" si="2"/>
         <v>101</v>
@@ -3520,15 +4141,15 @@
         <v>def hab_esp_101(dato, personaje):</v>
       </c>
     </row>
-    <row r="201" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F201" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="203" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E203">
-        <f t="shared" ref="E201:E225" si="3">E200+1</f>
+        <f t="shared" ref="E203:E224" si="3">E200+1</f>
         <v>102</v>
       </c>
       <c r="F203" t="str">
@@ -3536,13 +4157,13 @@
         <v>def hab_esp_102(dato, personaje):</v>
       </c>
     </row>
-    <row r="204" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F204" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="206" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E206">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -3552,13 +4173,13 @@
         <v>def hab_esp_103(dato, personaje):</v>
       </c>
     </row>
-    <row r="207" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F207" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="209" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E209">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -3568,13 +4189,13 @@
         <v>def hab_esp_104(dato, personaje):</v>
       </c>
     </row>
-    <row r="210" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F210" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="212" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E212">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -3584,13 +4205,13 @@
         <v>def hab_esp_105(dato, personaje):</v>
       </c>
     </row>
-    <row r="213" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F213" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="215" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E215">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -3600,13 +4221,13 @@
         <v>def hab_esp_106(dato, personaje):</v>
       </c>
     </row>
-    <row r="216" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F216" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="218" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E218">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -3616,13 +4237,13 @@
         <v>def hab_esp_107(dato, personaje):</v>
       </c>
     </row>
-    <row r="219" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F219" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="221" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E221">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -3632,13 +4253,13 @@
         <v>def hab_esp_108(dato, personaje):</v>
       </c>
     </row>
-    <row r="222" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="5:6" x14ac:dyDescent="0.25">
       <c r="F222" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
-    <row r="224" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E224">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -3648,14 +4269,14 @@
         <v>def hab_esp_109(dato, personaje):</v>
       </c>
     </row>
-    <row r="225" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F225" t="str">
         <f>$B$3</f>
         <v>    return</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E2:F225" xr:uid="{A2E82D6E-79FB-4501-BC6E-470E9C5171A2}"/>
+  <autoFilter ref="E2:F225"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>